<commit_message>
importer: ignore null rows
</commit_message>
<xml_diff>
--- a/DataPortalCare/src/test/resources/ProofExampleFull.xlsx
+++ b/DataPortalCare/src/test/resources/ProofExampleFull.xlsx
@@ -141,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -164,11 +164,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -183,6 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -487,10 +499,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,6 +1470,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L26" s="8">
+        <v>5556</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>